<commit_message>
Update Count in file
</commit_message>
<xml_diff>
--- a/Quotes Report_Res2.xlsx
+++ b/Quotes Report_Res2.xlsx
@@ -423,7 +423,7 @@
         <v>24</v>
       </c>
       <c r="B3" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4">
@@ -431,7 +431,7 @@
         <v>25</v>
       </c>
       <c r="B4" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5">
@@ -439,7 +439,7 @@
         <v>26</v>
       </c>
       <c r="B5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
create report after 100 calls
</commit_message>
<xml_diff>
--- a/Quotes Report_Res2.xlsx
+++ b/Quotes Report_Res2.xlsx
@@ -415,7 +415,7 @@
         <v>23</v>
       </c>
       <c r="B2" t="n">
-        <v>5</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3">
@@ -423,7 +423,7 @@
         <v>24</v>
       </c>
       <c r="B3" t="n">
-        <v>4</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4">
@@ -431,7 +431,7 @@
         <v>25</v>
       </c>
       <c r="B4" t="n">
-        <v>11</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5">
@@ -439,7 +439,7 @@
         <v>26</v>
       </c>
       <c r="B5" t="n">
-        <v>3</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>